<commit_message>
Feat: Implement PyQt6 dashboard, refine reporting logic, and finalize build config
MAJOR CHANGES:
- GUI: Replaced text console with a floating PyQt6 dashboard (audit_gui.py) featuring Start/Abort controls and progress tracking.
- UX: Added logic to offset the dashboard window 450px to the right to prevent blocking the Laserfiche login screen.
- Reporting: Updated generation logic to timestamp the audit (K34/K35), highlight/clear dead links, and remove hyperlinks.

BUILD & CONFIG:
- PyInstaller: Updated path handling to support "frozen" EXE state and renamed browser dependency folder to '_sys_core' for protection.
- Cleanup: Updated .gitignore to exclude build artifacts (dist/build) and deleted deprecated scripts (gui_app.py).
- Docs: Added project README.md.
</commit_message>
<xml_diff>
--- a/Kinnex Revision Source.xlsx
+++ b/Kinnex Revision Source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\RevisionAuditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F933F2D8-1F58-42AB-BF89-C5D20AFCDEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EAE595-6DB1-47FD-8F32-07B108B4356E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5FB7ED20-4720-41E5-81F8-3AA616E5495D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
   <si>
     <t>WI-03-081</t>
   </si>
@@ -219,16 +219,13 @@
     <t>KNX0251</t>
   </si>
   <si>
-    <t>If any cells are highlighted, revisions were detected. The link will take you to a page that says "entry not found." Manually update 'Kinnex Revision Checker' before running the macro again. Instructions on Sheet2</t>
-  </si>
-  <si>
     <t>2. Open "Kinnex Revision Checker" worksheet, NOT "Kinnex Revisions" worksheet.</t>
   </si>
   <si>
-    <t>Login to Laserfiche before running the macro!</t>
-  </si>
-  <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>If any cells are highlighted, revisions were detected. Manually update the hyperlink for 'Kinnex Revision Source' before running the app again.</t>
   </si>
 </sst>
 </file>
@@ -238,7 +235,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,12 +278,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -629,7 +620,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
@@ -641,13 +632,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
@@ -659,7 +650,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
@@ -681,10 +672,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -693,56 +684,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -762,84 +753,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
-          <xdr:row>35</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>638175</xdr:colOff>
-          <xdr:row>38</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Button 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Aptos Narrow"/>
-                </a:rPr>
-                <a:t>Revision Check Macro</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2384,12 +2298,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0149B4A2-54C3-4F11-A66E-C5EDF430A27A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0149B4A2-54C3-4F11-A66E-C5EDF430A27A}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2416,13 +2330,13 @@
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
       <c r="F1" s="7"/>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="60"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="58"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
@@ -2435,11 +2349,11 @@
       </c>
       <c r="E2" s="47"/>
       <c r="F2" s="36"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="55"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -2458,20 +2372,20 @@
         <v>44272</v>
       </c>
       <c r="F3" s="37"/>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="52"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="50"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="15">
         <v>45971</v>
@@ -2483,11 +2397,11 @@
         <v>45875</v>
       </c>
       <c r="F4" s="37"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="55"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
@@ -3116,13 +3030,13 @@
       <c r="D29" s="2"/>
       <c r="E29" s="15"/>
       <c r="F29" s="38"/>
-      <c r="G29" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
-      <c r="K29" s="57"/>
+      <c r="G29" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="55"/>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
@@ -3131,11 +3045,11 @@
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
       <c r="F30" s="37"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
-      <c r="K30" s="57"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="55"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
@@ -3144,11 +3058,11 @@
       <c r="D31" s="2"/>
       <c r="E31" s="15"/>
       <c r="F31" s="37"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="57"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="55"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
@@ -3157,32 +3071,32 @@
       <c r="D32" s="2"/>
       <c r="E32" s="15"/>
       <c r="F32" s="37"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="57"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="55"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="F33" s="37"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="57"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="55"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
       <c r="F34" s="37"/>
-      <c r="G34" s="61" t="s">
+      <c r="G34" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="59"/>
+      <c r="J34" s="59"/>
       <c r="K34" s="18"/>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3197,11 +3111,9 @@
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
       <c r="F36" s="37"/>
-      <c r="G36" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="63"/>
       <c r="J36" s="40"/>
       <c r="K36" s="20"/>
     </row>
@@ -3210,18 +3122,18 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="F37" s="37"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="63"/>
       <c r="J37" s="40"/>
       <c r="K37" s="20"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="F38" s="37"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
       <c r="J38" s="40"/>
       <c r="K38" s="20"/>
     </row>
@@ -3232,17 +3144,16 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="13"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="64"/>
+      <c r="I39" s="64"/>
       <c r="J39" s="14"/>
       <c r="K39" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G36:I39"/>
     <mergeCell ref="G3:K4"/>
     <mergeCell ref="G29:K33"/>
     <mergeCell ref="B2:C2"/>
@@ -3292,36 +3203,6 @@
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId37"/>
-  <drawing r:id="rId38"/>
-  <legacyDrawing r:id="rId39"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId40" name="Button 1">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!ExtractChromeTabRev">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>9</xdr:col>
-                    <xdr:colOff>66675</xdr:colOff>
-                    <xdr:row>35</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>10</xdr:col>
-                    <xdr:colOff>638175</xdr:colOff>
-                    <xdr:row>38</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -3330,38 +3211,38 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:W122"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A96" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="64"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="62"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -3505,31 +3386,31 @@
       <c r="W31" s="24"/>
     </row>
     <row r="32" spans="1:23" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="63"/>
-      <c r="O32" s="63"/>
-      <c r="P32" s="63"/>
-      <c r="Q32" s="63"/>
-      <c r="R32" s="63"/>
-      <c r="S32" s="63"/>
-      <c r="T32" s="63"/>
-      <c r="U32" s="63"/>
-      <c r="V32" s="63"/>
-      <c r="W32" s="64"/>
+      <c r="A32" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="61"/>
+      <c r="P32" s="61"/>
+      <c r="Q32" s="61"/>
+      <c r="R32" s="61"/>
+      <c r="S32" s="61"/>
+      <c r="T32" s="61"/>
+      <c r="U32" s="61"/>
+      <c r="V32" s="61"/>
+      <c r="W32" s="62"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
@@ -3630,31 +3511,31 @@
       <c r="W46" s="28"/>
     </row>
     <row r="47" spans="1:23" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="62" t="s">
+      <c r="A47" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
-      <c r="G47" s="63"/>
-      <c r="H47" s="63"/>
-      <c r="I47" s="63"/>
-      <c r="J47" s="63"/>
-      <c r="K47" s="63"/>
-      <c r="L47" s="63"/>
-      <c r="M47" s="63"/>
-      <c r="N47" s="63"/>
-      <c r="O47" s="63"/>
-      <c r="P47" s="63"/>
-      <c r="Q47" s="63"/>
-      <c r="R47" s="63"/>
-      <c r="S47" s="63"/>
-      <c r="T47" s="63"/>
-      <c r="U47" s="63"/>
-      <c r="V47" s="63"/>
-      <c r="W47" s="64"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="61"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="61"/>
+      <c r="L47" s="61"/>
+      <c r="M47" s="61"/>
+      <c r="N47" s="61"/>
+      <c r="O47" s="61"/>
+      <c r="P47" s="61"/>
+      <c r="Q47" s="61"/>
+      <c r="R47" s="61"/>
+      <c r="S47" s="61"/>
+      <c r="T47" s="61"/>
+      <c r="U47" s="61"/>
+      <c r="V47" s="61"/>
+      <c r="W47" s="62"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
@@ -3742,31 +3623,31 @@
       <c r="W63" s="17"/>
     </row>
     <row r="64" spans="1:23" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="62" t="s">
+      <c r="A64" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="63"/>
-      <c r="C64" s="63"/>
-      <c r="D64" s="63"/>
-      <c r="E64" s="63"/>
-      <c r="F64" s="63"/>
-      <c r="G64" s="63"/>
-      <c r="H64" s="63"/>
-      <c r="I64" s="63"/>
-      <c r="J64" s="63"/>
-      <c r="K64" s="63"/>
-      <c r="L64" s="63"/>
-      <c r="M64" s="63"/>
-      <c r="N64" s="63"/>
-      <c r="O64" s="63"/>
-      <c r="P64" s="63"/>
-      <c r="Q64" s="63"/>
-      <c r="R64" s="63"/>
-      <c r="S64" s="63"/>
-      <c r="T64" s="63"/>
-      <c r="U64" s="63"/>
-      <c r="V64" s="63"/>
-      <c r="W64" s="64"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="61"/>
+      <c r="D64" s="61"/>
+      <c r="E64" s="61"/>
+      <c r="F64" s="61"/>
+      <c r="G64" s="61"/>
+      <c r="H64" s="61"/>
+      <c r="I64" s="61"/>
+      <c r="J64" s="61"/>
+      <c r="K64" s="61"/>
+      <c r="L64" s="61"/>
+      <c r="M64" s="61"/>
+      <c r="N64" s="61"/>
+      <c r="O64" s="61"/>
+      <c r="P64" s="61"/>
+      <c r="Q64" s="61"/>
+      <c r="R64" s="61"/>
+      <c r="S64" s="61"/>
+      <c r="T64" s="61"/>
+      <c r="U64" s="61"/>
+      <c r="V64" s="61"/>
+      <c r="W64" s="62"/>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="25"/>
@@ -3862,31 +3743,31 @@
       <c r="W82" s="17"/>
     </row>
     <row r="83" spans="1:23" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="62" t="s">
+      <c r="A83" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B83" s="63"/>
-      <c r="C83" s="63"/>
-      <c r="D83" s="63"/>
-      <c r="E83" s="63"/>
-      <c r="F83" s="63"/>
-      <c r="G83" s="63"/>
-      <c r="H83" s="63"/>
-      <c r="I83" s="63"/>
-      <c r="J83" s="63"/>
-      <c r="K83" s="63"/>
-      <c r="L83" s="63"/>
-      <c r="M83" s="63"/>
-      <c r="N83" s="63"/>
-      <c r="O83" s="63"/>
-      <c r="P83" s="63"/>
-      <c r="Q83" s="63"/>
-      <c r="R83" s="63"/>
-      <c r="S83" s="63"/>
-      <c r="T83" s="63"/>
-      <c r="U83" s="63"/>
-      <c r="V83" s="63"/>
-      <c r="W83" s="64"/>
+      <c r="B83" s="61"/>
+      <c r="C83" s="61"/>
+      <c r="D83" s="61"/>
+      <c r="E83" s="61"/>
+      <c r="F83" s="61"/>
+      <c r="G83" s="61"/>
+      <c r="H83" s="61"/>
+      <c r="I83" s="61"/>
+      <c r="J83" s="61"/>
+      <c r="K83" s="61"/>
+      <c r="L83" s="61"/>
+      <c r="M83" s="61"/>
+      <c r="N83" s="61"/>
+      <c r="O83" s="61"/>
+      <c r="P83" s="61"/>
+      <c r="Q83" s="61"/>
+      <c r="R83" s="61"/>
+      <c r="S83" s="61"/>
+      <c r="T83" s="61"/>
+      <c r="U83" s="61"/>
+      <c r="V83" s="61"/>
+      <c r="W83" s="62"/>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" s="25"/>
@@ -3990,31 +3871,31 @@
       <c r="W103" s="17"/>
     </row>
     <row r="104" spans="1:23" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="62" t="s">
+      <c r="A104" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B104" s="63"/>
-      <c r="C104" s="63"/>
-      <c r="D104" s="63"/>
-      <c r="E104" s="63"/>
-      <c r="F104" s="63"/>
-      <c r="G104" s="63"/>
-      <c r="H104" s="63"/>
-      <c r="I104" s="63"/>
-      <c r="J104" s="63"/>
-      <c r="K104" s="63"/>
-      <c r="L104" s="63"/>
-      <c r="M104" s="63"/>
-      <c r="N104" s="63"/>
-      <c r="O104" s="63"/>
-      <c r="P104" s="63"/>
-      <c r="Q104" s="63"/>
-      <c r="R104" s="63"/>
-      <c r="S104" s="63"/>
-      <c r="T104" s="63"/>
-      <c r="U104" s="63"/>
-      <c r="V104" s="63"/>
-      <c r="W104" s="64"/>
+      <c r="B104" s="61"/>
+      <c r="C104" s="61"/>
+      <c r="D104" s="61"/>
+      <c r="E104" s="61"/>
+      <c r="F104" s="61"/>
+      <c r="G104" s="61"/>
+      <c r="H104" s="61"/>
+      <c r="I104" s="61"/>
+      <c r="J104" s="61"/>
+      <c r="K104" s="61"/>
+      <c r="L104" s="61"/>
+      <c r="M104" s="61"/>
+      <c r="N104" s="61"/>
+      <c r="O104" s="61"/>
+      <c r="P104" s="61"/>
+      <c r="Q104" s="61"/>
+      <c r="R104" s="61"/>
+      <c r="S104" s="61"/>
+      <c r="T104" s="61"/>
+      <c r="U104" s="61"/>
+      <c r="V104" s="61"/>
+      <c r="W104" s="62"/>
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" s="8"/>

</xml_diff>